<commit_message>
free_y parameter added to spreadsheet.
</commit_message>
<xml_diff>
--- a/Reserve_Level_Template/figure_files/Reserve_Level_Plotting_Variables.xlsx
+++ b/Reserve_Level_Template/figure_files/Reserve_Level_Plotting_Variables.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jpadilla\Desktop\template_prep\Final_Reports\Reserve_Level_Template\figure_files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dave.Eslinger\Documents\GitHub\SWMP_Status_Reports\Reserve_Level_Template\figure_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11985" tabRatio="829" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11988" tabRatio="829" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Global_Decisions--&gt;" sheetId="7" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="382" uniqueCount="108">
   <si>
     <t>Flags</t>
   </si>
@@ -354,12 +354,15 @@
   </si>
   <si>
     <t>Include station labels on trend maps?</t>
+  </si>
+  <si>
+    <t>Free_Y</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -683,7 +686,7 @@
       <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -697,14 +700,14 @@
       <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.44140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="22" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>24</v>
       </c>
@@ -724,7 +727,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>27</v>
       </c>
@@ -732,7 +735,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>28</v>
       </c>
@@ -740,7 +743,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>29</v>
       </c>
@@ -760,7 +763,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>30</v>
       </c>
@@ -768,7 +771,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>31</v>
       </c>
@@ -776,7 +779,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>102</v>
       </c>
@@ -784,7 +787,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>39</v>
       </c>
@@ -792,7 +795,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>40</v>
       </c>
@@ -800,7 +803,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>41</v>
       </c>
@@ -808,7 +811,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>42</v>
       </c>
@@ -816,7 +819,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>43</v>
       </c>
@@ -824,7 +827,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>44</v>
       </c>
@@ -832,7 +835,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>45</v>
       </c>
@@ -840,7 +843,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>48</v>
       </c>
@@ -854,7 +857,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>49</v>
       </c>
@@ -862,7 +865,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>50</v>
       </c>
@@ -870,7 +873,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>51</v>
       </c>
@@ -878,7 +881,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>52</v>
       </c>
@@ -886,7 +889,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>53</v>
       </c>
@@ -900,7 +903,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>54</v>
       </c>
@@ -914,7 +917,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>55</v>
       </c>
@@ -941,32 +944,32 @@
       <selection activeCell="O10" sqref="N10:O10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>104</v>
       </c>
@@ -984,12 +987,12 @@
       <selection activeCell="G34" sqref="G34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -997,7 +1000,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>2007</v>
       </c>
@@ -1005,7 +1008,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2016</v>
       </c>
@@ -1023,23 +1026,23 @@
       <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.5703125" customWidth="1"/>
-    <col min="3" max="3" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.5546875" customWidth="1"/>
+    <col min="3" max="3" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -1062,7 +1065,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -1076,7 +1079,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -1090,7 +1093,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -1104,7 +1107,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -1118,7 +1121,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -1132,7 +1135,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -1146,7 +1149,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -1160,7 +1163,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -1174,7 +1177,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -1188,7 +1191,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -1202,7 +1205,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>18</v>
       </c>
@@ -1216,7 +1219,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>19</v>
       </c>
@@ -1230,7 +1233,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>72</v>
       </c>
@@ -1251,15 +1254,15 @@
       <selection sqref="A1:A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="18.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>76</v>
       </c>
@@ -1276,7 +1279,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>-121.79810000000001</v>
       </c>
@@ -1293,7 +1296,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>36.847099999999998</v>
       </c>
@@ -1307,7 +1310,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>-121.71939999999999</v>
       </c>
@@ -1321,7 +1324,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>36.795699999999997</v>
       </c>
@@ -1335,7 +1338,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>73</v>
       </c>
@@ -1349,16 +1352,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="49.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="49.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>57</v>
       </c>
@@ -1366,7 +1369,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>78</v>
       </c>
@@ -1374,7 +1377,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>79</v>
       </c>
@@ -1382,7 +1385,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>103</v>
       </c>
@@ -1390,7 +1393,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>59</v>
       </c>
@@ -1398,7 +1401,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>60</v>
       </c>
@@ -1406,7 +1409,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>77</v>
       </c>
@@ -1414,7 +1417,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>100</v>
       </c>
@@ -1422,7 +1425,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>101</v>
       </c>
@@ -1430,7 +1433,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>105</v>
       </c>
@@ -1438,7 +1441,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>106</v>
       </c>
@@ -1462,7 +1465,7 @@
       <selection activeCell="G33" sqref="G33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1470,24 +1473,24 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E22"/>
+  <dimension ref="A1:F22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1:F22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.7109375" customWidth="1"/>
-    <col min="5" max="5" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="31.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.6640625" customWidth="1"/>
+    <col min="5" max="5" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.44140625" customWidth="1"/>
     <col min="7" max="7" width="29" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>24</v>
       </c>
@@ -1503,8 +1506,11 @@
       <c r="E1" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>27</v>
       </c>
@@ -1517,8 +1523,11 @@
       <c r="D2" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>28</v>
       </c>
@@ -1531,8 +1540,11 @@
       <c r="D3" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>29</v>
       </c>
@@ -1548,8 +1560,11 @@
       <c r="E4">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>30</v>
       </c>
@@ -1562,8 +1577,11 @@
       <c r="D5" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>31</v>
       </c>
@@ -1576,8 +1594,11 @@
       <c r="D6" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F6" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>102</v>
       </c>
@@ -1590,8 +1611,11 @@
       <c r="D7" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>39</v>
       </c>
@@ -1604,8 +1628,11 @@
       <c r="D8" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F8" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>40</v>
       </c>
@@ -1618,8 +1645,11 @@
       <c r="D9" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F9" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>41</v>
       </c>
@@ -1632,8 +1662,11 @@
       <c r="D10" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F10" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>42</v>
       </c>
@@ -1646,8 +1679,11 @@
       <c r="D11" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F11" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>43</v>
       </c>
@@ -1660,8 +1696,11 @@
       <c r="D12" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F12" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>44</v>
       </c>
@@ -1674,8 +1713,11 @@
       <c r="D13" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F13" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>45</v>
       </c>
@@ -1688,8 +1730,11 @@
       <c r="D14" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F14" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>48</v>
       </c>
@@ -1702,8 +1747,11 @@
       <c r="D15" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F15" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>49</v>
       </c>
@@ -1716,8 +1764,11 @@
       <c r="D16" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F16" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>50</v>
       </c>
@@ -1730,8 +1781,11 @@
       <c r="D17" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F17" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>51</v>
       </c>
@@ -1744,8 +1798,11 @@
       <c r="D18" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F18" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>52</v>
       </c>
@@ -1758,8 +1815,11 @@
       <c r="D19" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F19" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>53</v>
       </c>
@@ -1772,8 +1832,11 @@
       <c r="D20" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F20" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>54</v>
       </c>
@@ -1786,8 +1849,11 @@
       <c r="D21" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F21" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>55</v>
       </c>
@@ -1798,6 +1864,9 @@
         <v>97</v>
       </c>
       <c r="D22" t="s">
+        <v>34</v>
+      </c>
+      <c r="F22" t="s">
         <v>34</v>
       </c>
     </row>
@@ -1814,19 +1883,19 @@
       <selection activeCell="N7" sqref="N7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="8" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="11" width="17.85546875" customWidth="1"/>
-    <col min="12" max="12" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="8" width="17.88671875" bestFit="1" customWidth="1"/>
+    <col min="9" max="11" width="17.88671875" customWidth="1"/>
+    <col min="12" max="12" width="16.44140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17.33203125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>24</v>
       </c>
@@ -1870,7 +1939,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>27</v>
       </c>
@@ -1890,7 +1959,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>28</v>
       </c>
@@ -1910,7 +1979,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>29</v>
       </c>
@@ -1951,7 +2020,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>30</v>
       </c>
@@ -1971,7 +2040,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>31</v>
       </c>
@@ -1988,7 +2057,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>102</v>
       </c>
@@ -2008,7 +2077,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>39</v>
       </c>
@@ -2028,7 +2097,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>40</v>
       </c>
@@ -2048,7 +2117,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>41</v>
       </c>
@@ -2068,7 +2137,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>42</v>
       </c>
@@ -2088,7 +2157,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>43</v>
       </c>
@@ -2108,7 +2177,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>44</v>
       </c>
@@ -2122,7 +2191,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>45</v>
       </c>
@@ -2136,7 +2205,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>48</v>
       </c>
@@ -2177,7 +2246,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>49</v>
       </c>
@@ -2197,7 +2266,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>50</v>
       </c>
@@ -2217,7 +2286,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>51</v>
       </c>
@@ -2237,7 +2306,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>52</v>
       </c>
@@ -2257,7 +2326,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>53</v>
       </c>
@@ -2298,7 +2367,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>54</v>
       </c>
@@ -2339,7 +2408,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>55</v>
       </c>

</xml_diff>